<commit_message>
Add poverty example data
Also fixes population data and provides convenient make-all.R file for
recreating data sets when changes are made to Excel files.
</commit_message>
<xml_diff>
--- a/data-raw/statepop.xlsx
+++ b/data-raw/statepop.xlsx
@@ -41,9 +41,6 @@
     <t>full</t>
   </si>
   <si>
-    <t>pop_est_2015</t>
-  </si>
-  <si>
     <t>AL</t>
   </si>
   <si>
@@ -501,6 +498,9 @@
   </si>
   <si>
     <t>56</t>
+  </si>
+  <si>
+    <t>pop_2015</t>
   </si>
 </sst>
 </file>
@@ -830,7 +830,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -838,7 +838,7 @@
     <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -852,18 +852,18 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
       <c r="D2" s="1">
         <v>4858979</v>
@@ -871,13 +871,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
       </c>
       <c r="D3" s="1">
         <v>738432</v>
@@ -885,13 +885,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
         <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
       </c>
       <c r="D4" s="1">
         <v>6828065</v>
@@ -899,13 +899,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
         <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
       </c>
       <c r="D5" s="1">
         <v>2978204</v>
@@ -913,13 +913,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
         <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
       </c>
       <c r="D6" s="1">
         <v>39144818</v>
@@ -927,13 +927,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
         <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
       </c>
       <c r="D7" s="1">
         <v>5456574</v>
@@ -941,13 +941,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
         <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
       </c>
       <c r="D8" s="1">
         <v>3590886</v>
@@ -955,13 +955,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
         <v>18</v>
-      </c>
-      <c r="C9" t="s">
-        <v>19</v>
       </c>
       <c r="D9" s="1">
         <v>945934</v>
@@ -969,13 +969,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
         <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>21</v>
       </c>
       <c r="D10" s="1">
         <v>672228</v>
@@ -983,13 +983,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
         <v>22</v>
-      </c>
-      <c r="C11" t="s">
-        <v>23</v>
       </c>
       <c r="D11" s="1">
         <v>20271272</v>
@@ -997,13 +997,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
         <v>24</v>
-      </c>
-      <c r="C12" t="s">
-        <v>25</v>
       </c>
       <c r="D12" s="1">
         <v>10214860</v>
@@ -1011,13 +1011,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
         <v>26</v>
-      </c>
-      <c r="C13" t="s">
-        <v>27</v>
       </c>
       <c r="D13" s="1">
         <v>1431603</v>
@@ -1025,13 +1025,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
         <v>28</v>
-      </c>
-      <c r="C14" t="s">
-        <v>29</v>
       </c>
       <c r="D14" s="1">
         <v>1654930</v>
@@ -1039,13 +1039,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
         <v>30</v>
-      </c>
-      <c r="C15" t="s">
-        <v>31</v>
       </c>
       <c r="D15" s="1">
         <v>12859995</v>
@@ -1053,13 +1053,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" t="s">
         <v>32</v>
-      </c>
-      <c r="C16" t="s">
-        <v>33</v>
       </c>
       <c r="D16" s="1">
         <v>6619680</v>
@@ -1067,13 +1067,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" t="s">
         <v>34</v>
-      </c>
-      <c r="C17" t="s">
-        <v>35</v>
       </c>
       <c r="D17" s="1">
         <v>3123899</v>
@@ -1081,13 +1081,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="s">
         <v>36</v>
-      </c>
-      <c r="C18" t="s">
-        <v>37</v>
       </c>
       <c r="D18" s="1">
         <v>2911641</v>
@@ -1095,13 +1095,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" t="s">
         <v>38</v>
-      </c>
-      <c r="C19" t="s">
-        <v>39</v>
       </c>
       <c r="D19" s="1">
         <v>4425092</v>
@@ -1109,13 +1109,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
         <v>40</v>
-      </c>
-      <c r="C20" t="s">
-        <v>41</v>
       </c>
       <c r="D20" s="1">
         <v>4670724</v>
@@ -1123,13 +1123,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" t="s">
         <v>42</v>
-      </c>
-      <c r="C21" t="s">
-        <v>43</v>
       </c>
       <c r="D21" s="1">
         <v>1329328</v>
@@ -1137,13 +1137,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" t="s">
         <v>44</v>
-      </c>
-      <c r="C22" t="s">
-        <v>45</v>
       </c>
       <c r="D22" s="1">
         <v>6006401</v>
@@ -1151,13 +1151,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" t="s">
         <v>46</v>
-      </c>
-      <c r="C23" t="s">
-        <v>47</v>
       </c>
       <c r="D23" s="1">
         <v>6794422</v>
@@ -1165,13 +1165,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" t="s">
         <v>48</v>
-      </c>
-      <c r="C24" t="s">
-        <v>49</v>
       </c>
       <c r="D24" s="1">
         <v>9922576</v>
@@ -1179,13 +1179,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" t="s">
         <v>50</v>
-      </c>
-      <c r="C25" t="s">
-        <v>51</v>
       </c>
       <c r="D25" s="1">
         <v>5489594</v>
@@ -1193,13 +1193,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" t="s">
         <v>52</v>
-      </c>
-      <c r="C26" t="s">
-        <v>53</v>
       </c>
       <c r="D26" s="1">
         <v>2992333</v>
@@ -1207,13 +1207,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" t="s">
         <v>54</v>
-      </c>
-      <c r="C27" t="s">
-        <v>55</v>
       </c>
       <c r="D27" s="1">
         <v>6083672</v>
@@ -1221,13 +1221,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" t="s">
         <v>56</v>
-      </c>
-      <c r="C28" t="s">
-        <v>57</v>
       </c>
       <c r="D28" s="1">
         <v>1032949</v>
@@ -1235,13 +1235,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" t="s">
         <v>58</v>
-      </c>
-      <c r="C29" t="s">
-        <v>59</v>
       </c>
       <c r="D29" s="1">
         <v>1896190</v>
@@ -1249,13 +1249,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B30" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" t="s">
         <v>60</v>
-      </c>
-      <c r="C30" t="s">
-        <v>61</v>
       </c>
       <c r="D30" s="1">
         <v>2890845</v>
@@ -1263,13 +1263,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B31" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" t="s">
         <v>62</v>
-      </c>
-      <c r="C31" t="s">
-        <v>63</v>
       </c>
       <c r="D31" s="1">
         <v>1330608</v>
@@ -1277,13 +1277,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B32" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" t="s">
         <v>64</v>
-      </c>
-      <c r="C32" t="s">
-        <v>65</v>
       </c>
       <c r="D32" s="1">
         <v>8958013</v>
@@ -1291,13 +1291,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" t="s">
         <v>66</v>
-      </c>
-      <c r="C33" t="s">
-        <v>67</v>
       </c>
       <c r="D33" s="1">
         <v>2085109</v>
@@ -1305,13 +1305,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B34" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" t="s">
         <v>68</v>
-      </c>
-      <c r="C34" t="s">
-        <v>69</v>
       </c>
       <c r="D34" s="1">
         <v>19795791</v>
@@ -1319,13 +1319,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B35" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" t="s">
         <v>70</v>
-      </c>
-      <c r="C35" t="s">
-        <v>71</v>
       </c>
       <c r="D35" s="1">
         <v>10042802</v>
@@ -1333,13 +1333,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" t="s">
         <v>72</v>
-      </c>
-      <c r="C36" t="s">
-        <v>73</v>
       </c>
       <c r="D36" s="1">
         <v>756927</v>
@@ -1347,13 +1347,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B37" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" t="s">
         <v>74</v>
-      </c>
-      <c r="C37" t="s">
-        <v>75</v>
       </c>
       <c r="D37" s="1">
         <v>11613423</v>
@@ -1361,13 +1361,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B38" t="s">
+        <v>75</v>
+      </c>
+      <c r="C38" t="s">
         <v>76</v>
-      </c>
-      <c r="C38" t="s">
-        <v>77</v>
       </c>
       <c r="D38" s="1">
         <v>3911338</v>
@@ -1375,13 +1375,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B39" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39" t="s">
         <v>78</v>
-      </c>
-      <c r="C39" t="s">
-        <v>79</v>
       </c>
       <c r="D39" s="1">
         <v>4028977</v>
@@ -1389,13 +1389,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B40" t="s">
+        <v>79</v>
+      </c>
+      <c r="C40" t="s">
         <v>80</v>
-      </c>
-      <c r="C40" t="s">
-        <v>81</v>
       </c>
       <c r="D40" s="1">
         <v>12802503</v>
@@ -1403,13 +1403,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B41" t="s">
+        <v>81</v>
+      </c>
+      <c r="C41" t="s">
         <v>82</v>
-      </c>
-      <c r="C41" t="s">
-        <v>83</v>
       </c>
       <c r="D41" s="1">
         <v>1056298</v>
@@ -1417,13 +1417,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B42" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42" t="s">
         <v>84</v>
-      </c>
-      <c r="C42" t="s">
-        <v>85</v>
       </c>
       <c r="D42" s="1">
         <v>4896146</v>
@@ -1431,13 +1431,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B43" t="s">
+        <v>85</v>
+      </c>
+      <c r="C43" t="s">
         <v>86</v>
-      </c>
-      <c r="C43" t="s">
-        <v>87</v>
       </c>
       <c r="D43" s="1">
         <v>858469</v>
@@ -1445,13 +1445,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B44" t="s">
+        <v>87</v>
+      </c>
+      <c r="C44" t="s">
         <v>88</v>
-      </c>
-      <c r="C44" t="s">
-        <v>89</v>
       </c>
       <c r="D44" s="1">
         <v>6600299</v>
@@ -1459,13 +1459,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B45" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45" t="s">
         <v>90</v>
-      </c>
-      <c r="C45" t="s">
-        <v>91</v>
       </c>
       <c r="D45" s="1">
         <v>27469114</v>
@@ -1473,13 +1473,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B46" t="s">
+        <v>91</v>
+      </c>
+      <c r="C46" t="s">
         <v>92</v>
-      </c>
-      <c r="C46" t="s">
-        <v>93</v>
       </c>
       <c r="D46" s="1">
         <v>2995919</v>
@@ -1487,13 +1487,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B47" t="s">
+        <v>93</v>
+      </c>
+      <c r="C47" t="s">
         <v>94</v>
-      </c>
-      <c r="C47" t="s">
-        <v>95</v>
       </c>
       <c r="D47" s="1">
         <v>626042</v>
@@ -1501,13 +1501,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B48" t="s">
+        <v>95</v>
+      </c>
+      <c r="C48" t="s">
         <v>96</v>
-      </c>
-      <c r="C48" t="s">
-        <v>97</v>
       </c>
       <c r="D48" s="1">
         <v>8382993</v>
@@ -1515,13 +1515,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B49" t="s">
+        <v>97</v>
+      </c>
+      <c r="C49" t="s">
         <v>98</v>
-      </c>
-      <c r="C49" t="s">
-        <v>99</v>
       </c>
       <c r="D49" s="1">
         <v>7170351</v>
@@ -1529,13 +1529,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B50" t="s">
+        <v>99</v>
+      </c>
+      <c r="C50" t="s">
         <v>100</v>
-      </c>
-      <c r="C50" t="s">
-        <v>101</v>
       </c>
       <c r="D50" s="1">
         <v>1844128</v>
@@ -1543,13 +1543,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B51" t="s">
+        <v>101</v>
+      </c>
+      <c r="C51" t="s">
         <v>102</v>
-      </c>
-      <c r="C51" t="s">
-        <v>103</v>
       </c>
       <c r="D51" s="1">
         <v>5771337</v>
@@ -1557,13 +1557,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B52" t="s">
+        <v>103</v>
+      </c>
+      <c r="C52" t="s">
         <v>104</v>
-      </c>
-      <c r="C52" t="s">
-        <v>105</v>
       </c>
       <c r="D52" s="1">
         <v>586107</v>

</xml_diff>